<commit_message>
upate write to excel to remove headers for easier data analysis
</commit_message>
<xml_diff>
--- a/BC_SVM_poly.xlsx
+++ b/BC_SVM_poly.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="11520" yWindow="4965" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7245" yWindow="4815" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Score" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,20 +11,25 @@
     <sheet name="CR" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -38,12 +43,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -56,9 +76,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -458,10 +481,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A7"/>
+  <dimension ref="A2:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -475,31 +498,22 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>0.9473684210526315</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>0.956140350877193</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>Score</t>
-        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.9736842105263158</v>
+        <v>0.9035087719298246</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Score</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>0.956140350877193</v>
+      <c r="A6" t="n">
+        <v>0.9385964912280702</v>
       </c>
     </row>
   </sheetData>
@@ -513,25 +527,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B10"/>
+  <dimension ref="A2:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D29" sqref="A1:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -539,23 +553,23 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -563,23 +577,23 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -587,10 +601,34 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>38</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>66</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>7</v>
+      </c>
+      <c r="B13" t="n">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -604,10 +642,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E19"/>
+  <dimension ref="A2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -635,26 +673,26 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9375</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.967741935483871</v>
+        <v>0.96</v>
       </c>
       <c r="E3" t="n">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -663,303 +701,354 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8717948717948718</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9315068493150684</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="E4" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.956140350877193</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="C5" t="n">
-        <v>0.956140350877193</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="D5" t="n">
-        <v>0.956140350877193</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="E5" t="n">
-        <v>0.956140350877193</v>
+        <v>0.9473684210526315</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>macro avg</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.96875</v>
+        <v>0.9615384615384616</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9358974358974359</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9496243923994697</v>
+        <v>0.9415384615384615</v>
       </c>
       <c r="E6" t="n">
         <v>114</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>weighted avg</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9588815789473685</v>
+        <v>0.9514170040485831</v>
       </c>
       <c r="C7" t="n">
-        <v>0.956140350877193</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9553457217945438</v>
+        <v>0.9463967611336033</v>
       </c>
       <c r="E7" t="n">
         <v>114</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>precision</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>recall</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>f1-score</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="inlineStr">
-        <is>
-          <t>support</t>
-        </is>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9315068493150684</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.9645390070921985</v>
+      </c>
+      <c r="E8" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.961038961038961</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0.8913043478260869</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9801324503311258</v>
+        <v>0.9425287356321839</v>
       </c>
       <c r="E9" t="n">
-        <v>74</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>accuracy</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0.956140350877193</v>
       </c>
       <c r="C10" t="n">
-        <v>0.925</v>
+        <v>0.956140350877193</v>
       </c>
       <c r="D10" t="n">
-        <v>0.961038961038961</v>
+        <v>0.956140350877193</v>
       </c>
       <c r="E10" t="n">
-        <v>40</v>
+        <v>0.956140350877193</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>accuracy</t>
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>macro avg</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9736842105263158</v>
+        <v>0.9657534246575342</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9736842105263158</v>
+        <v>0.9456521739130435</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9736842105263158</v>
+        <v>0.9535338713621913</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9736842105263158</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>macro avg</t>
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>weighted avg</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9805194805194806</v>
+        <v>0.9591444364335495</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9625</v>
+        <v>0.956140350877193</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9705857056850434</v>
+        <v>0.9556576694855259</v>
       </c>
       <c r="E12" t="n">
         <v>114</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8625</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.9261744966442953</v>
+      </c>
+      <c r="E13" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.7555555555555555</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.8607594936708861</v>
+      </c>
+      <c r="E14" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9035087719298246</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9035087719298246</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9035087719298246</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.9035087719298246</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>macro avg</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.93125</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8777777777777778</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.8934669951575906</v>
+      </c>
+      <c r="E16" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>weighted avg</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>0.9747095010252905</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9736842105263158</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9734329804040505</v>
-      </c>
-      <c r="E13" t="n">
+      <c r="B17" t="n">
+        <v>0.9167763157894737</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.9035087719298246</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.9003527849442653</v>
+      </c>
+      <c r="E17" t="n">
         <v>114</v>
       </c>
     </row>
-    <row r="14">
-      <c r="B14" s="1" t="inlineStr">
-        <is>
-          <t>precision</t>
-        </is>
-      </c>
-      <c r="C14" s="1" t="inlineStr">
-        <is>
-          <t>recall</t>
-        </is>
-      </c>
-      <c r="D14" s="1" t="inlineStr">
-        <is>
-          <t>f1-score</t>
-        </is>
-      </c>
-      <c r="E14" s="1" t="inlineStr">
-        <is>
-          <t>support</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>0.9342105263157895</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.9659863945578231</v>
-      </c>
-      <c r="E15" t="n">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="B18" t="n">
+        <v>0.9041095890410958</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.9496402877697842</v>
+      </c>
+      <c r="E18" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0.8837209302325582</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.9382716049382716</v>
-      </c>
-      <c r="E16" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.8541666666666666</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.9213483146067416</v>
+      </c>
+      <c r="E19" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>accuracy</t>
         </is>
       </c>
-      <c r="B17" t="n">
-        <v>0.956140350877193</v>
-      </c>
-      <c r="C17" t="n">
-        <v>0.956140350877193</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.956140350877193</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.956140350877193</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
+      <c r="B20" t="n">
+        <v>0.9385964912280702</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9385964912280702</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.9385964912280702</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.9385964912280702</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>macro avg</t>
         </is>
       </c>
-      <c r="B18" t="n">
-        <v>0.9671052631578947</v>
-      </c>
-      <c r="C18" t="n">
-        <v>0.9418604651162791</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0.9521289997480473</v>
-      </c>
-      <c r="E18" t="n">
+      <c r="B21" t="n">
+        <v>0.952054794520548</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.9270833333333333</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.9354943011882628</v>
+      </c>
+      <c r="E21" t="n">
         <v>114</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>weighted avg</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>0.9590258541089566</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.956140350877193</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0.95553257040308</v>
-      </c>
-      <c r="E19" t="n">
+      <c r="B22" t="n">
+        <v>0.9444844989185291</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.9385964912280702</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.9377278780169241</v>
+      </c>
+      <c r="E22" t="n">
         <v>114</v>
       </c>
     </row>

</xml_diff>